<commit_message>
updating menlo park to menlo park, ca
</commit_message>
<xml_diff>
--- a/data/resume.xlsx
+++ b/data/resume.xlsx
@@ -100,7 +100,7 @@
     <t>GRAIL</t>
   </si>
   <si>
-    <t>Menlo Park</t>
+    <t>Menlo Park, CA</t>
   </si>
   <si>
     <t>February 2021</t>
@@ -640,7 +640,7 @@
       <c r="D4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="1" t="s">

</xml_diff>

<commit_message>
fixing grad year to text
</commit_message>
<xml_diff>
--- a/data/resume.xlsx
+++ b/data/resume.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>section</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Irvine, CA</t>
+  </si>
+  <si>
+    <t>2018</t>
   </si>
   <si>
     <t>Major in Mathematics</t>
@@ -268,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -277,6 +280,9 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -608,14 +614,14 @@
       <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1">
-        <v>2018.0</v>
+      <c r="G3" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -629,91 +635,91 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="Q4" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="R4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="b">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -724,49 +730,49 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="b">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="M6" s="6" t="s">
         <v>62</v>
       </c>
+      <c r="N6" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="O6" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -774,13 +780,13 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -795,16 +801,16 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B8" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>68</v>
+      <c r="I8" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -818,13 +824,13 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B9" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -839,13 +845,13 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B10" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>

</xml_diff>